<commit_message>
- Eoi print preview and commitment-letter added
</commit_message>
<xml_diff>
--- a/storage/app/wsps.xlsx
+++ b/storage/app/wsps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/CLSG/storage/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FBA818-F287-5447-9C07-84AF1C853255}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D162C0-CCC4-734D-929C-5D37756788F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{EDA3B495-3E64-7E41-A6F2-917CEA41AECA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>PostalCode</t>
+  </si>
+  <si>
+    <t>ManagingDirector</t>
   </si>
 </sst>
 </file>
@@ -132,14 +135,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{551C1DC3-AEC0-5B4C-A71B-AF254E1D3469}" name="Table1" displayName="Table1" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F1048576" xr:uid="{A2720B3F-1089-F545-9D1C-29409829888D}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{551C1DC3-AEC0-5B4C-A71B-AF254E1D3469}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G1048576" xr:uid="{A2720B3F-1089-F545-9D1C-29409829888D}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B68CB258-6B70-C047-A26B-C3F8F9CEC6E9}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2A299B77-9412-D74E-B663-831C1B0DC9F7}" name="Acronym"/>
     <tableColumn id="3" xr3:uid="{D229B32B-C3CC-6747-8076-6238ACB9946E}" name="Email"/>
     <tableColumn id="4" xr3:uid="{61FFA6F0-5FA2-3B41-85E9-ABA58973DA16}" name="PostalAddress"/>
     <tableColumn id="5" xr3:uid="{E404111C-7A48-034D-A396-6957FE50CEFF}" name="PhysicalAddress"/>
+    <tableColumn id="7" xr3:uid="{6F16390B-7E0D-E446-B257-408303A9D0C1}" name="ManagingDirector"/>
     <tableColumn id="6" xr3:uid="{600D3E03-E402-AF42-B3D9-3C2506CCA92E}" name="PostalCode"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -443,20 +447,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD4119B-E20F-2547-8BBC-7AEAC46EC681}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="5" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,6 +477,9 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Remove keep-alive - Add managing director to excel export - Add import wsp to dashboard
</commit_message>
<xml_diff>
--- a/storage/app/wsps.xlsx
+++ b/storage/app/wsps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/CLSG/storage/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D162C0-CCC4-734D-929C-5D37756788F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF5E182-E391-3E41-B98F-BC36BBBFE63F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{EDA3B495-3E64-7E41-A6F2-917CEA41AECA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>ManagingDirector</t>
+  </si>
+  <si>
+    <t>MangingDirector</t>
   </si>
 </sst>
 </file>
@@ -135,9 +138,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{551C1DC3-AEC0-5B4C-A71B-AF254E1D3469}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:G1048576" xr:uid="{A2720B3F-1089-F545-9D1C-29409829888D}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{551C1DC3-AEC0-5B4C-A71B-AF254E1D3469}" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:H1048576" xr:uid="{A2720B3F-1089-F545-9D1C-29409829888D}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B68CB258-6B70-C047-A26B-C3F8F9CEC6E9}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2A299B77-9412-D74E-B663-831C1B0DC9F7}" name="Acronym"/>
     <tableColumn id="3" xr3:uid="{D229B32B-C3CC-6747-8076-6238ACB9946E}" name="Email"/>
@@ -145,6 +148,7 @@
     <tableColumn id="5" xr3:uid="{E404111C-7A48-034D-A396-6957FE50CEFF}" name="PhysicalAddress"/>
     <tableColumn id="7" xr3:uid="{6F16390B-7E0D-E446-B257-408303A9D0C1}" name="ManagingDirector"/>
     <tableColumn id="6" xr3:uid="{600D3E03-E402-AF42-B3D9-3C2506CCA92E}" name="PostalCode"/>
+    <tableColumn id="8" xr3:uid="{90E9092E-7E43-D84A-BC7C-C4748ADA6FF9}" name="MangingDirector"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -447,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD4119B-E20F-2547-8BBC-7AEAC46EC681}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -458,9 +462,10 @@
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,6 +486,9 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add self assign eoi,bcp,erp
</commit_message>
<xml_diff>
--- a/storage/app/wsps.xlsx
+++ b/storage/app/wsps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/CLSG/storage/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF5E182-E391-3E41-B98F-BC36BBBFE63F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5F7E07-F424-2640-B1EB-B58C97A8BEE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{EDA3B495-3E64-7E41-A6F2-917CEA41AECA}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{EDA3B495-3E64-7E41-A6F2-917CEA41AECA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>ManagingDirector</t>
-  </si>
-  <si>
-    <t>MangingDirector</t>
   </si>
 </sst>
 </file>
@@ -138,9 +135,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{551C1DC3-AEC0-5B4C-A71B-AF254E1D3469}" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:H1048576" xr:uid="{A2720B3F-1089-F545-9D1C-29409829888D}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{551C1DC3-AEC0-5B4C-A71B-AF254E1D3469}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G1048576" xr:uid="{A2720B3F-1089-F545-9D1C-29409829888D}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B68CB258-6B70-C047-A26B-C3F8F9CEC6E9}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2A299B77-9412-D74E-B663-831C1B0DC9F7}" name="Acronym"/>
     <tableColumn id="3" xr3:uid="{D229B32B-C3CC-6747-8076-6238ACB9946E}" name="Email"/>
@@ -148,7 +145,6 @@
     <tableColumn id="5" xr3:uid="{E404111C-7A48-034D-A396-6957FE50CEFF}" name="PhysicalAddress"/>
     <tableColumn id="7" xr3:uid="{6F16390B-7E0D-E446-B257-408303A9D0C1}" name="ManagingDirector"/>
     <tableColumn id="6" xr3:uid="{600D3E03-E402-AF42-B3D9-3C2506CCA92E}" name="PostalCode"/>
-    <tableColumn id="8" xr3:uid="{90E9092E-7E43-D84A-BC7C-C4748ADA6FF9}" name="MangingDirector"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -451,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD4119B-E20F-2547-8BBC-7AEAC46EC681}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -462,10 +458,9 @@
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="11.1640625" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,9 +481,6 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>